<commit_message>
#10 allow string to be used for output (which means it can be used as derived)
</commit_message>
<xml_diff>
--- a/resources/parameters.xlsx
+++ b/resources/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlhumber/iiipy/stoolbox/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B2490E-C540-BE43-A477-B0B77F5F85A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287DE46B-576D-054B-802F-05474521F811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="1140" windowWidth="30240" windowHeight="18880" xr2:uid="{C9864FCB-DD2E-D646-9669-B24A34CEB34F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C9864FCB-DD2E-D646-9669-B24A34CEB34F}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -2641,9 +2641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12499223-B988-D14D-92DB-90E19BB713F2}">
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5717,7 +5715,7 @@
         <v>568</v>
       </c>
       <c r="G118" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H118" t="s">
         <v>348</v>

</xml_diff>

<commit_message>
#30 include Time Units and Network Travel Mode
</commit_message>
<xml_diff>
--- a/resources/parameters.xlsx
+++ b/resources/parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlhumber/iiipy/stoolbox/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlhumber/iiipy/autobox/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287DE46B-576D-054B-802F-05474521F811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421864DF-3A66-E74B-8114-56C5E9712215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C9864FCB-DD2E-D646-9669-B24A34CEB34F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="576">
   <si>
     <t>3D Tiles Layer</t>
   </si>
@@ -1758,6 +1758,9 @@
   </si>
   <si>
     <t>v0.1.0</t>
+  </si>
+  <si>
+    <t>v0.2.0</t>
   </si>
 </sst>
 </file>
@@ -2641,7 +2644,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12499223-B988-D14D-92DB-90E19BB713F2}">
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4877,10 +4882,10 @@
         <v>251</v>
       </c>
       <c r="E86" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F86" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G86" t="s">
         <v>569</v>
@@ -5917,10 +5922,10 @@
         <v>544</v>
       </c>
       <c r="E126" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F126" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G126" t="s">
         <v>569</v>

</xml_diff>

<commit_message>
#32 include some additional parameters
</commit_message>
<xml_diff>
--- a/resources/parameters.xlsx
+++ b/resources/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlhumber/iiipy/autobox/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421864DF-3A66-E74B-8114-56C5E9712215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACAE817-99A2-AF46-8E3C-389DC5E9150A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C9864FCB-DD2E-D646-9669-B24A34CEB34F}"/>
   </bookViews>
@@ -2644,9 +2644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12499223-B988-D14D-92DB-90E19BB713F2}">
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3660,10 +3658,10 @@
         <v>459</v>
       </c>
       <c r="E39" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F39" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G39" t="s">
         <v>569</v>
@@ -3946,10 +3944,10 @@
         <v>464</v>
       </c>
       <c r="E50" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F50" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G50" t="s">
         <v>568</v>
@@ -4804,10 +4802,10 @@
         <v>507</v>
       </c>
       <c r="E83" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F83" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G83" t="s">
         <v>568</v>
@@ -4856,10 +4854,10 @@
         <v>509</v>
       </c>
       <c r="E85" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F85" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G85" t="s">
         <v>568</v>
@@ -5324,10 +5322,10 @@
         <v>524</v>
       </c>
       <c r="E103" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F103" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G103" t="s">
         <v>569</v>

</xml_diff>

<commit_message>
#35 include more parameter types
</commit_message>
<xml_diff>
--- a/resources/parameters.xlsx
+++ b/resources/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlhumber/iiipy/autobox/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACAE817-99A2-AF46-8E3C-389DC5E9150A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD50C52-FF19-0549-9BCF-FDF08929BF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C9864FCB-DD2E-D646-9669-B24A34CEB34F}"/>
   </bookViews>
@@ -1767,7 +1767,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1898,6 +1898,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2084,7 +2091,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2199,6 +2206,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF44B3E1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF44B3E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2244,8 +2262,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2644,7 +2663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12499223-B988-D14D-92DB-90E19BB713F2}">
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3059,11 +3080,11 @@
       <c r="D16" t="s">
         <v>451</v>
       </c>
-      <c r="E16" t="s">
-        <v>573</v>
-      </c>
-      <c r="F16" t="s">
-        <v>569</v>
+      <c r="E16" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G16" t="s">
         <v>569</v>
@@ -3216,10 +3237,10 @@
         <v>453</v>
       </c>
       <c r="E22" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F22" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G22" t="s">
         <v>568</v>
@@ -3372,10 +3393,10 @@
         <v>454</v>
       </c>
       <c r="E28" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F28" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G28" t="s">
         <v>568</v>
@@ -3553,11 +3574,11 @@
       <c r="D35" t="s">
         <v>457</v>
       </c>
-      <c r="E35" t="s">
-        <v>573</v>
-      </c>
-      <c r="F35" t="s">
-        <v>569</v>
+      <c r="E35" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G35" t="s">
         <v>569</v>
@@ -3710,10 +3731,10 @@
         <v>460</v>
       </c>
       <c r="E41" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F41" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G41" t="s">
         <v>569</v>
@@ -3735,11 +3756,11 @@
       <c r="D42" t="s">
         <v>461</v>
       </c>
-      <c r="E42" t="s">
-        <v>573</v>
-      </c>
-      <c r="F42" t="s">
-        <v>569</v>
+      <c r="E42" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G42" t="s">
         <v>569</v>
@@ -3839,11 +3860,11 @@
       <c r="D46" t="s">
         <v>463</v>
       </c>
-      <c r="E46" t="s">
-        <v>573</v>
-      </c>
-      <c r="F46" t="s">
-        <v>569</v>
+      <c r="E46" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G46" t="s">
         <v>569</v>
@@ -3866,10 +3887,10 @@
         <v>486</v>
       </c>
       <c r="E47" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F47" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G47" t="s">
         <v>569</v>
@@ -3918,10 +3939,10 @@
         <v>487</v>
       </c>
       <c r="E49" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F49" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G49" t="s">
         <v>568</v>
@@ -3969,11 +3990,11 @@
       <c r="D51" t="s">
         <v>465</v>
       </c>
-      <c r="E51" t="s">
-        <v>573</v>
-      </c>
-      <c r="F51" t="s">
-        <v>569</v>
+      <c r="E51" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G51" t="s">
         <v>569</v>
@@ -3996,10 +4017,10 @@
         <v>466</v>
       </c>
       <c r="E52" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F52" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G52" t="s">
         <v>569</v>
@@ -4151,11 +4172,11 @@
       <c r="D58" t="s">
         <v>490</v>
       </c>
-      <c r="E58" t="s">
-        <v>573</v>
-      </c>
-      <c r="F58" t="s">
-        <v>569</v>
+      <c r="E58" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G58" t="s">
         <v>569</v>
@@ -4333,11 +4354,11 @@
       <c r="D65" t="s">
         <v>496</v>
       </c>
-      <c r="E65" t="s">
-        <v>573</v>
-      </c>
-      <c r="F65" t="s">
-        <v>569</v>
+      <c r="E65" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G65" t="s">
         <v>568</v>
@@ -4542,10 +4563,10 @@
         <v>500</v>
       </c>
       <c r="E73" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F73" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G73" t="s">
         <v>569</v>
@@ -4697,11 +4718,11 @@
       <c r="D79" t="s">
         <v>504</v>
       </c>
-      <c r="E79" t="s">
-        <v>573</v>
-      </c>
-      <c r="F79" t="s">
-        <v>569</v>
+      <c r="E79" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G79" t="s">
         <v>569</v>
@@ -4723,11 +4744,11 @@
       <c r="D80" t="s">
         <v>233</v>
       </c>
-      <c r="E80" t="s">
-        <v>573</v>
-      </c>
-      <c r="F80" t="s">
-        <v>569</v>
+      <c r="E80" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G80" t="s">
         <v>569</v>
@@ -4749,11 +4770,11 @@
       <c r="D81" t="s">
         <v>505</v>
       </c>
-      <c r="E81" t="s">
-        <v>573</v>
-      </c>
-      <c r="F81" t="s">
-        <v>569</v>
+      <c r="E81" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G81" t="s">
         <v>569</v>
@@ -4775,11 +4796,11 @@
       <c r="D82" t="s">
         <v>506</v>
       </c>
-      <c r="E82" t="s">
-        <v>573</v>
-      </c>
-      <c r="F82" t="s">
-        <v>569</v>
+      <c r="E82" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G82" t="s">
         <v>568</v>
@@ -5061,11 +5082,11 @@
       <c r="D93" t="s">
         <v>514</v>
       </c>
-      <c r="E93" t="s">
-        <v>573</v>
-      </c>
-      <c r="F93" t="s">
-        <v>569</v>
+      <c r="E93" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G93" t="s">
         <v>569</v>
@@ -5087,11 +5108,11 @@
       <c r="D94" t="s">
         <v>515</v>
       </c>
-      <c r="E94" t="s">
-        <v>573</v>
-      </c>
-      <c r="F94" t="s">
-        <v>569</v>
+      <c r="E94" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G94" t="s">
         <v>569</v>
@@ -5114,10 +5135,10 @@
         <v>516</v>
       </c>
       <c r="E95" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F95" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G95" t="s">
         <v>569</v>
@@ -5269,11 +5290,11 @@
       <c r="D101" t="s">
         <v>522</v>
       </c>
-      <c r="E101" t="s">
-        <v>573</v>
-      </c>
-      <c r="F101" t="s">
-        <v>569</v>
+      <c r="E101" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G101" t="s">
         <v>569</v>
@@ -5296,10 +5317,10 @@
         <v>523</v>
       </c>
       <c r="E102" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F102" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G102" t="s">
         <v>569</v>
@@ -5374,10 +5395,10 @@
         <v>526</v>
       </c>
       <c r="E105" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F105" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G105" t="s">
         <v>569</v>
@@ -5452,10 +5473,10 @@
         <v>529</v>
       </c>
       <c r="E108" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F108" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G108" t="s">
         <v>568</v>
@@ -5478,13 +5499,13 @@
         <v>530</v>
       </c>
       <c r="E109" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F109" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G109" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H109" t="s">
         <v>321</v>
@@ -5504,13 +5525,13 @@
         <v>531</v>
       </c>
       <c r="E110" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F110" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G110" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H110" t="s">
         <v>324</v>
@@ -5530,13 +5551,13 @@
         <v>532</v>
       </c>
       <c r="E111" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F111" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G111" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H111" t="s">
         <v>327</v>
@@ -5556,13 +5577,13 @@
         <v>533</v>
       </c>
       <c r="E112" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F112" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G112" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H112" t="s">
         <v>330</v>
@@ -5582,10 +5603,10 @@
         <v>534</v>
       </c>
       <c r="E113" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F113" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G113" t="s">
         <v>569</v>
@@ -5816,10 +5837,10 @@
         <v>540</v>
       </c>
       <c r="E122" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F122" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G122" t="s">
         <v>568</v>
@@ -5867,11 +5888,11 @@
       <c r="D124" t="s">
         <v>542</v>
       </c>
-      <c r="E124" t="s">
-        <v>573</v>
-      </c>
-      <c r="F124" t="s">
-        <v>569</v>
+      <c r="E124" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G124" t="s">
         <v>569</v>
@@ -5893,11 +5914,11 @@
       <c r="D125" t="s">
         <v>543</v>
       </c>
-      <c r="E125" t="s">
-        <v>573</v>
-      </c>
-      <c r="F125" t="s">
-        <v>569</v>
+      <c r="E125" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G125" t="s">
         <v>569</v>
@@ -6049,11 +6070,11 @@
       <c r="D131" t="s">
         <v>547</v>
       </c>
-      <c r="E131" t="s">
-        <v>573</v>
-      </c>
-      <c r="F131" t="s">
-        <v>569</v>
+      <c r="E131" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G131" t="s">
         <v>569</v>
@@ -6102,10 +6123,10 @@
         <v>548</v>
       </c>
       <c r="E133" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F133" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G133" t="s">
         <v>568</v>
@@ -6127,11 +6148,11 @@
       <c r="D134" t="s">
         <v>549</v>
       </c>
-      <c r="E134" t="s">
-        <v>573</v>
-      </c>
-      <c r="F134" t="s">
-        <v>569</v>
+      <c r="E134" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G134" t="s">
         <v>569</v>
@@ -6232,10 +6253,10 @@
         <v>553</v>
       </c>
       <c r="E138" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F138" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G138" t="s">
         <v>569</v>
@@ -6283,11 +6304,11 @@
       <c r="D140" t="s">
         <v>554</v>
       </c>
-      <c r="E140" t="s">
-        <v>573</v>
-      </c>
-      <c r="F140" t="s">
-        <v>569</v>
+      <c r="E140" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G140" t="s">
         <v>568</v>
@@ -6309,11 +6330,11 @@
       <c r="D141" t="s">
         <v>555</v>
       </c>
-      <c r="E141" t="s">
-        <v>573</v>
-      </c>
-      <c r="F141" t="s">
-        <v>569</v>
+      <c r="E141" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G141" t="s">
         <v>569</v>
@@ -6413,11 +6434,11 @@
       <c r="D145" t="s">
         <v>559</v>
       </c>
-      <c r="E145" t="s">
-        <v>573</v>
-      </c>
-      <c r="F145" t="s">
-        <v>569</v>
+      <c r="E145" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G145" t="s">
         <v>569</v>
@@ -6439,11 +6460,11 @@
       <c r="D146" t="s">
         <v>560</v>
       </c>
-      <c r="E146" t="s">
-        <v>573</v>
-      </c>
-      <c r="F146" t="s">
-        <v>569</v>
+      <c r="E146" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="G146" t="s">
         <v>569</v>
@@ -6518,10 +6539,10 @@
         <v>562</v>
       </c>
       <c r="E149" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F149" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G149" t="s">
         <v>569</v>
@@ -6544,10 +6565,10 @@
         <v>563</v>
       </c>
       <c r="E150" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="F150" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G150" t="s">
         <v>569</v>

</xml_diff>

<commit_message>
#36 flag double and long as output, add UPDATED column to store version
</commit_message>
<xml_diff>
--- a/resources/parameters.xlsx
+++ b/resources/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlhumber/iiipy/autobox/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD50C52-FF19-0549-9BCF-FDF08929BF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19F438D-F886-6445-8DF2-7E4718F27DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C9864FCB-DD2E-D646-9669-B24A34CEB34F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="577">
   <si>
     <t>3D Tiles Layer</t>
   </si>
@@ -1761,6 +1761,9 @@
   </si>
   <si>
     <t>v0.2.0</t>
+  </si>
+  <si>
+    <t>UPDATED</t>
   </si>
 </sst>
 </file>
@@ -2328,14 +2331,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF301D14-8247-894B-83A9-D7C37C6859A8}" name="Table1" displayName="Table1" ref="A1:H150" totalsRowShown="0">
-  <autoFilter ref="A1:H150" xr:uid="{DF301D14-8247-894B-83A9-D7C37C6859A8}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF301D14-8247-894B-83A9-D7C37C6859A8}" name="Table1" displayName="Table1" ref="A1:I150" totalsRowShown="0">
+  <autoFilter ref="A1:I150" xr:uid="{DF301D14-8247-894B-83A9-D7C37C6859A8}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8B6495D5-11CD-FA46-B617-46B522A0B4D8}" name="ORDER"/>
     <tableColumn id="2" xr3:uid="{71A5C3DF-2D88-DC42-A61D-CE93A584FECB}" name="NAME"/>
     <tableColumn id="3" xr3:uid="{3427CE42-BFC7-6446-9450-C6BCAA15742F}" name="KEYWORD"/>
     <tableColumn id="4" xr3:uid="{386C2ACF-2FC4-BF42-9942-9903DBF7D071}" name="CLASS"/>
     <tableColumn id="7" xr3:uid="{FCBB7E64-CDD9-4542-80CB-3E44954689E4}" name="VERSION" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{76B933F9-B2CB-224B-85E4-A2D57BD1B754}" name="UPDATED"/>
     <tableColumn id="5" xr3:uid="{B2B5419D-33EE-0A4A-B541-CEB1AF3F78ED}" name="GENERATE"/>
     <tableColumn id="8" xr3:uid="{207E3DC1-9ECC-944D-A8E4-143BD1093FED}" name="OUTPUT"/>
     <tableColumn id="6" xr3:uid="{E785CCEB-3B5D-3A4B-A6C4-B3C043C423F2}" name="COMMENT"/>
@@ -2661,11 +2665,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12499223-B988-D14D-92DB-90E19BB713F2}">
-  <dimension ref="A1:H150"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2673,11 +2675,12 @@
     <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.83203125" customWidth="1"/>
-    <col min="8" max="8" width="192" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="192" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>467</v>
       </c>
@@ -2694,16 +2697,19 @@
         <v>572</v>
       </c>
       <c r="F1" t="s">
+        <v>576</v>
+      </c>
+      <c r="G1" t="s">
         <v>567</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>570</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2719,17 +2725,17 @@
       <c r="E2" t="s">
         <v>573</v>
       </c>
-      <c r="F2" t="s">
-        <v>569</v>
-      </c>
       <c r="G2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H2" t="s">
+        <v>568</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2745,17 +2751,17 @@
       <c r="E3" t="s">
         <v>573</v>
       </c>
-      <c r="F3" t="s">
-        <v>569</v>
-      </c>
       <c r="G3" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H3" t="s">
+        <v>568</v>
+      </c>
+      <c r="I3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2771,17 +2777,17 @@
       <c r="E4" t="s">
         <v>574</v>
       </c>
-      <c r="F4" t="s">
-        <v>568</v>
-      </c>
       <c r="G4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H4" t="s">
+        <v>569</v>
+      </c>
+      <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2797,17 +2803,17 @@
       <c r="E5" t="s">
         <v>573</v>
       </c>
-      <c r="F5" t="s">
-        <v>569</v>
-      </c>
       <c r="G5" t="s">
         <v>569</v>
       </c>
       <c r="H5" t="s">
+        <v>569</v>
+      </c>
+      <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2823,17 +2829,17 @@
       <c r="E6" t="s">
         <v>574</v>
       </c>
-      <c r="F6" t="s">
-        <v>568</v>
-      </c>
       <c r="G6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H6" t="s">
+        <v>569</v>
+      </c>
+      <c r="I6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2849,17 +2855,17 @@
       <c r="E7" t="s">
         <v>574</v>
       </c>
-      <c r="F7" t="s">
-        <v>568</v>
-      </c>
       <c r="G7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H7" t="s">
+        <v>569</v>
+      </c>
+      <c r="I7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2875,17 +2881,17 @@
       <c r="E8" t="s">
         <v>574</v>
       </c>
-      <c r="F8" t="s">
-        <v>568</v>
-      </c>
       <c r="G8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H8" t="s">
+        <v>569</v>
+      </c>
+      <c r="I8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2901,17 +2907,17 @@
       <c r="E9" t="s">
         <v>574</v>
       </c>
-      <c r="F9" t="s">
-        <v>568</v>
-      </c>
       <c r="G9" t="s">
         <v>568</v>
       </c>
       <c r="H9" t="s">
+        <v>568</v>
+      </c>
+      <c r="I9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2927,17 +2933,17 @@
       <c r="E10" t="s">
         <v>574</v>
       </c>
-      <c r="F10" t="s">
-        <v>568</v>
-      </c>
       <c r="G10" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H10" t="s">
+        <v>569</v>
+      </c>
+      <c r="I10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2953,17 +2959,17 @@
       <c r="E11" t="s">
         <v>574</v>
       </c>
-      <c r="F11" t="s">
-        <v>568</v>
-      </c>
       <c r="G11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H11" t="s">
+        <v>569</v>
+      </c>
+      <c r="I11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2979,17 +2985,17 @@
       <c r="E12" t="s">
         <v>573</v>
       </c>
-      <c r="F12" t="s">
-        <v>569</v>
-      </c>
       <c r="G12" t="s">
         <v>569</v>
       </c>
       <c r="H12" t="s">
+        <v>569</v>
+      </c>
+      <c r="I12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3005,17 +3011,17 @@
       <c r="E13" t="s">
         <v>574</v>
       </c>
-      <c r="F13" t="s">
-        <v>568</v>
-      </c>
       <c r="G13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H13" t="s">
+        <v>569</v>
+      </c>
+      <c r="I13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3031,17 +3037,17 @@
       <c r="E14" t="s">
         <v>574</v>
       </c>
-      <c r="F14" t="s">
-        <v>568</v>
-      </c>
       <c r="G14" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H14" t="s">
+        <v>569</v>
+      </c>
+      <c r="I14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3057,17 +3063,17 @@
       <c r="E15" t="s">
         <v>573</v>
       </c>
-      <c r="F15" t="s">
-        <v>569</v>
-      </c>
       <c r="G15" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H15" t="s">
+        <v>568</v>
+      </c>
+      <c r="I15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3083,17 +3089,18 @@
       <c r="E16" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G16" t="s">
-        <v>569</v>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H16" t="s">
+        <v>569</v>
+      </c>
+      <c r="I16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3109,17 +3116,17 @@
       <c r="E17" t="s">
         <v>574</v>
       </c>
-      <c r="F17" t="s">
-        <v>568</v>
-      </c>
       <c r="G17" t="s">
         <v>568</v>
       </c>
       <c r="H17" t="s">
+        <v>568</v>
+      </c>
+      <c r="I17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3135,17 +3142,17 @@
       <c r="E18" t="s">
         <v>573</v>
       </c>
-      <c r="F18" t="s">
-        <v>569</v>
-      </c>
       <c r="G18" t="s">
         <v>569</v>
       </c>
       <c r="H18" t="s">
+        <v>569</v>
+      </c>
+      <c r="I18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3161,17 +3168,17 @@
       <c r="E19" t="s">
         <v>574</v>
       </c>
-      <c r="F19" t="s">
-        <v>568</v>
-      </c>
       <c r="G19" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H19" t="s">
+        <v>569</v>
+      </c>
+      <c r="I19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3187,17 +3194,17 @@
       <c r="E20" t="s">
         <v>574</v>
       </c>
-      <c r="F20" t="s">
-        <v>568</v>
-      </c>
       <c r="G20" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H20" t="s">
+        <v>569</v>
+      </c>
+      <c r="I20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3213,17 +3220,17 @@
       <c r="E21" t="s">
         <v>574</v>
       </c>
-      <c r="F21" t="s">
-        <v>568</v>
-      </c>
       <c r="G21" t="s">
         <v>568</v>
       </c>
       <c r="H21" t="s">
+        <v>568</v>
+      </c>
+      <c r="I21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3239,17 +3246,17 @@
       <c r="E22" t="s">
         <v>575</v>
       </c>
-      <c r="F22" t="s">
-        <v>568</v>
-      </c>
       <c r="G22" t="s">
         <v>568</v>
       </c>
       <c r="H22" t="s">
+        <v>568</v>
+      </c>
+      <c r="I22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3265,17 +3272,17 @@
       <c r="E23" t="s">
         <v>573</v>
       </c>
-      <c r="F23" t="s">
-        <v>569</v>
-      </c>
       <c r="G23" t="s">
         <v>569</v>
       </c>
       <c r="H23" t="s">
+        <v>569</v>
+      </c>
+      <c r="I23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3291,17 +3298,17 @@
       <c r="E24" t="s">
         <v>574</v>
       </c>
-      <c r="F24" t="s">
-        <v>568</v>
-      </c>
       <c r="G24" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H24" t="s">
+        <v>569</v>
+      </c>
+      <c r="I24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3317,17 +3324,17 @@
       <c r="E25" t="s">
         <v>574</v>
       </c>
-      <c r="F25" t="s">
-        <v>568</v>
-      </c>
       <c r="G25" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H25" t="s">
+        <v>569</v>
+      </c>
+      <c r="I25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3343,17 +3350,17 @@
       <c r="E26" t="s">
         <v>574</v>
       </c>
-      <c r="F26" t="s">
-        <v>568</v>
-      </c>
       <c r="G26" t="s">
         <v>568</v>
       </c>
       <c r="H26" t="s">
+        <v>568</v>
+      </c>
+      <c r="I26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3369,17 +3376,17 @@
       <c r="E27" t="s">
         <v>573</v>
       </c>
-      <c r="F27" t="s">
-        <v>569</v>
-      </c>
       <c r="G27" t="s">
         <v>569</v>
       </c>
       <c r="H27" t="s">
+        <v>569</v>
+      </c>
+      <c r="I27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3395,17 +3402,17 @@
       <c r="E28" t="s">
         <v>575</v>
       </c>
-      <c r="F28" t="s">
-        <v>568</v>
-      </c>
       <c r="G28" t="s">
         <v>568</v>
       </c>
       <c r="H28" t="s">
+        <v>568</v>
+      </c>
+      <c r="I28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3421,17 +3428,17 @@
       <c r="E29" t="s">
         <v>573</v>
       </c>
-      <c r="F29" t="s">
-        <v>569</v>
-      </c>
       <c r="G29" t="s">
         <v>569</v>
       </c>
       <c r="H29" t="s">
+        <v>569</v>
+      </c>
+      <c r="I29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3448,16 +3455,19 @@
         <v>574</v>
       </c>
       <c r="F30" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="G30" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H30" t="s">
+        <v>568</v>
+      </c>
+      <c r="I30" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3473,17 +3483,17 @@
       <c r="E31" t="s">
         <v>574</v>
       </c>
-      <c r="F31" t="s">
-        <v>568</v>
-      </c>
       <c r="G31" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H31" t="s">
+        <v>569</v>
+      </c>
+      <c r="I31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3499,17 +3509,17 @@
       <c r="E32" t="s">
         <v>574</v>
       </c>
-      <c r="F32" t="s">
-        <v>568</v>
-      </c>
       <c r="G32" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H32" t="s">
+        <v>569</v>
+      </c>
+      <c r="I32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3525,17 +3535,17 @@
       <c r="E33" t="s">
         <v>573</v>
       </c>
-      <c r="F33" t="s">
-        <v>569</v>
-      </c>
       <c r="G33" t="s">
         <v>569</v>
       </c>
       <c r="H33" t="s">
+        <v>569</v>
+      </c>
+      <c r="I33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3551,17 +3561,17 @@
       <c r="E34" t="s">
         <v>574</v>
       </c>
-      <c r="F34" t="s">
-        <v>568</v>
-      </c>
       <c r="G34" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H34" t="s">
+        <v>569</v>
+      </c>
+      <c r="I34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3577,17 +3587,18 @@
       <c r="E35" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G35" t="s">
-        <v>569</v>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H35" t="s">
+        <v>569</v>
+      </c>
+      <c r="I35" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3603,17 +3614,17 @@
       <c r="E36" t="s">
         <v>574</v>
       </c>
-      <c r="F36" t="s">
-        <v>568</v>
-      </c>
       <c r="G36" t="s">
         <v>568</v>
       </c>
       <c r="H36" t="s">
+        <v>568</v>
+      </c>
+      <c r="I36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3629,17 +3640,17 @@
       <c r="E37" t="s">
         <v>574</v>
       </c>
-      <c r="F37" t="s">
-        <v>568</v>
-      </c>
       <c r="G37" t="s">
         <v>568</v>
       </c>
       <c r="H37" t="s">
+        <v>568</v>
+      </c>
+      <c r="I37" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3655,17 +3666,17 @@
       <c r="E38" t="s">
         <v>574</v>
       </c>
-      <c r="F38" t="s">
-        <v>568</v>
-      </c>
       <c r="G38" t="s">
         <v>568</v>
       </c>
       <c r="H38" t="s">
+        <v>568</v>
+      </c>
+      <c r="I38" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3681,17 +3692,17 @@
       <c r="E39" t="s">
         <v>575</v>
       </c>
-      <c r="F39" t="s">
-        <v>568</v>
-      </c>
       <c r="G39" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H39" t="s">
+        <v>569</v>
+      </c>
+      <c r="I39" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3707,17 +3718,17 @@
       <c r="E40" t="s">
         <v>574</v>
       </c>
-      <c r="F40" t="s">
-        <v>568</v>
-      </c>
       <c r="G40" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H40" t="s">
+        <v>569</v>
+      </c>
+      <c r="I40" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3733,17 +3744,17 @@
       <c r="E41" t="s">
         <v>575</v>
       </c>
-      <c r="F41" t="s">
-        <v>568</v>
-      </c>
       <c r="G41" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H41" t="s">
+        <v>569</v>
+      </c>
+      <c r="I41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3759,17 +3770,18 @@
       <c r="E42" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G42" t="s">
-        <v>569</v>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H42" t="s">
+        <v>569</v>
+      </c>
+      <c r="I42" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3785,17 +3797,17 @@
       <c r="E43" t="s">
         <v>574</v>
       </c>
-      <c r="F43" t="s">
-        <v>568</v>
-      </c>
       <c r="G43" t="s">
         <v>568</v>
       </c>
       <c r="H43" t="s">
+        <v>568</v>
+      </c>
+      <c r="I43" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3811,17 +3823,17 @@
       <c r="E44" t="s">
         <v>574</v>
       </c>
-      <c r="F44" t="s">
-        <v>568</v>
-      </c>
       <c r="G44" t="s">
         <v>568</v>
       </c>
       <c r="H44" t="s">
+        <v>568</v>
+      </c>
+      <c r="I44" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3837,17 +3849,17 @@
       <c r="E45" t="s">
         <v>573</v>
       </c>
-      <c r="F45" t="s">
-        <v>569</v>
-      </c>
       <c r="G45" t="s">
         <v>569</v>
       </c>
       <c r="H45" t="s">
+        <v>569</v>
+      </c>
+      <c r="I45" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3863,17 +3875,18 @@
       <c r="E46" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G46" t="s">
-        <v>569</v>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H46" t="s">
+        <v>569</v>
+      </c>
+      <c r="I46" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3889,17 +3902,17 @@
       <c r="E47" t="s">
         <v>575</v>
       </c>
-      <c r="F47" t="s">
-        <v>568</v>
-      </c>
       <c r="G47" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H47" t="s">
+        <v>569</v>
+      </c>
+      <c r="I47" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3915,17 +3928,17 @@
       <c r="E48" t="s">
         <v>573</v>
       </c>
-      <c r="F48" t="s">
-        <v>569</v>
-      </c>
       <c r="G48" t="s">
         <v>569</v>
       </c>
       <c r="H48" t="s">
+        <v>569</v>
+      </c>
+      <c r="I48" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3941,17 +3954,17 @@
       <c r="E49" t="s">
         <v>575</v>
       </c>
-      <c r="F49" t="s">
-        <v>568</v>
-      </c>
       <c r="G49" t="s">
         <v>568</v>
       </c>
       <c r="H49" t="s">
+        <v>568</v>
+      </c>
+      <c r="I49" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3967,17 +3980,17 @@
       <c r="E50" t="s">
         <v>575</v>
       </c>
-      <c r="F50" t="s">
-        <v>568</v>
-      </c>
       <c r="G50" t="s">
         <v>568</v>
       </c>
       <c r="H50" t="s">
+        <v>568</v>
+      </c>
+      <c r="I50" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3993,17 +4006,18 @@
       <c r="E51" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G51" t="s">
-        <v>569</v>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H51" t="s">
+        <v>569</v>
+      </c>
+      <c r="I51" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4019,17 +4033,17 @@
       <c r="E52" t="s">
         <v>575</v>
       </c>
-      <c r="F52" t="s">
-        <v>568</v>
-      </c>
       <c r="G52" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H52" t="s">
+        <v>569</v>
+      </c>
+      <c r="I52" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4045,17 +4059,17 @@
       <c r="E53" t="s">
         <v>573</v>
       </c>
-      <c r="F53" t="s">
-        <v>569</v>
-      </c>
       <c r="G53" t="s">
         <v>569</v>
       </c>
       <c r="H53" t="s">
+        <v>569</v>
+      </c>
+      <c r="I53" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4071,17 +4085,17 @@
       <c r="E54" t="s">
         <v>573</v>
       </c>
-      <c r="F54" t="s">
-        <v>569</v>
-      </c>
       <c r="G54" t="s">
         <v>569</v>
       </c>
       <c r="H54" t="s">
+        <v>569</v>
+      </c>
+      <c r="I54" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4097,17 +4111,17 @@
       <c r="E55" t="s">
         <v>573</v>
       </c>
-      <c r="F55" t="s">
-        <v>569</v>
-      </c>
       <c r="G55" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H55" t="s">
+        <v>568</v>
+      </c>
+      <c r="I55" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4123,17 +4137,17 @@
       <c r="E56" t="s">
         <v>573</v>
       </c>
-      <c r="F56" t="s">
-        <v>569</v>
-      </c>
       <c r="G56" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H56" t="s">
+        <v>568</v>
+      </c>
+      <c r="I56" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4149,17 +4163,17 @@
       <c r="E57" t="s">
         <v>574</v>
       </c>
-      <c r="F57" t="s">
-        <v>568</v>
-      </c>
       <c r="G57" t="s">
         <v>568</v>
       </c>
       <c r="H57" t="s">
+        <v>568</v>
+      </c>
+      <c r="I57" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4175,17 +4189,18 @@
       <c r="E58" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G58" t="s">
-        <v>569</v>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H58" t="s">
+        <v>569</v>
+      </c>
+      <c r="I58" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4201,17 +4216,17 @@
       <c r="E59" t="s">
         <v>573</v>
       </c>
-      <c r="F59" t="s">
-        <v>569</v>
-      </c>
       <c r="G59" t="s">
         <v>569</v>
       </c>
       <c r="H59" t="s">
+        <v>569</v>
+      </c>
+      <c r="I59" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4227,17 +4242,17 @@
       <c r="E60" t="s">
         <v>573</v>
       </c>
-      <c r="F60" t="s">
-        <v>569</v>
-      </c>
       <c r="G60" t="s">
         <v>569</v>
       </c>
       <c r="H60" t="s">
+        <v>569</v>
+      </c>
+      <c r="I60" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4253,17 +4268,17 @@
       <c r="E61" t="s">
         <v>573</v>
       </c>
-      <c r="F61" t="s">
-        <v>569</v>
-      </c>
       <c r="G61" t="s">
         <v>569</v>
       </c>
       <c r="H61" t="s">
+        <v>569</v>
+      </c>
+      <c r="I61" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4279,17 +4294,17 @@
       <c r="E62" t="s">
         <v>573</v>
       </c>
-      <c r="F62" t="s">
-        <v>569</v>
-      </c>
       <c r="G62" t="s">
         <v>569</v>
       </c>
       <c r="H62" t="s">
+        <v>569</v>
+      </c>
+      <c r="I62" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4305,17 +4320,17 @@
       <c r="E63" t="s">
         <v>573</v>
       </c>
-      <c r="F63" t="s">
-        <v>569</v>
-      </c>
       <c r="G63" t="s">
         <v>569</v>
       </c>
       <c r="H63" t="s">
+        <v>569</v>
+      </c>
+      <c r="I63" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4331,17 +4346,17 @@
       <c r="E64" t="s">
         <v>573</v>
       </c>
-      <c r="F64" t="s">
-        <v>569</v>
-      </c>
       <c r="G64" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H64" t="s">
+        <v>568</v>
+      </c>
+      <c r="I64" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4357,17 +4372,18 @@
       <c r="E65" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="F65" s="1"/>
+      <c r="G65" s="1" t="s">
         <v>568</v>
       </c>
       <c r="H65" t="s">
+        <v>568</v>
+      </c>
+      <c r="I65" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4383,17 +4399,17 @@
       <c r="E66" t="s">
         <v>574</v>
       </c>
-      <c r="F66" t="s">
-        <v>568</v>
-      </c>
       <c r="G66" t="s">
         <v>568</v>
       </c>
       <c r="H66" t="s">
+        <v>568</v>
+      </c>
+      <c r="I66" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4409,17 +4425,17 @@
       <c r="E67" t="s">
         <v>574</v>
       </c>
-      <c r="F67" t="s">
-        <v>568</v>
-      </c>
       <c r="G67" t="s">
         <v>568</v>
       </c>
       <c r="H67" t="s">
+        <v>568</v>
+      </c>
+      <c r="I67" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4435,17 +4451,17 @@
       <c r="E68" t="s">
         <v>574</v>
       </c>
-      <c r="F68" t="s">
-        <v>568</v>
-      </c>
       <c r="G68" t="s">
         <v>568</v>
       </c>
       <c r="H68" t="s">
+        <v>568</v>
+      </c>
+      <c r="I68" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4461,17 +4477,17 @@
       <c r="E69" t="s">
         <v>574</v>
       </c>
-      <c r="F69" t="s">
-        <v>568</v>
-      </c>
       <c r="G69" t="s">
         <v>568</v>
       </c>
       <c r="H69" t="s">
+        <v>568</v>
+      </c>
+      <c r="I69" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4487,17 +4503,17 @@
       <c r="E70" t="s">
         <v>573</v>
       </c>
-      <c r="F70" t="s">
-        <v>569</v>
-      </c>
       <c r="G70" t="s">
         <v>569</v>
       </c>
       <c r="H70" t="s">
+        <v>569</v>
+      </c>
+      <c r="I70" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4513,17 +4529,17 @@
       <c r="E71" t="s">
         <v>574</v>
       </c>
-      <c r="F71" t="s">
-        <v>568</v>
-      </c>
       <c r="G71" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H71" t="s">
+        <v>569</v>
+      </c>
+      <c r="I71" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4540,16 +4556,19 @@
         <v>574</v>
       </c>
       <c r="F72" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="G72" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H72" t="s">
+        <v>568</v>
+      </c>
+      <c r="I72" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4565,17 +4584,17 @@
       <c r="E73" t="s">
         <v>575</v>
       </c>
-      <c r="F73" t="s">
-        <v>568</v>
-      </c>
       <c r="G73" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H73" t="s">
+        <v>569</v>
+      </c>
+      <c r="I73" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4591,17 +4610,17 @@
       <c r="E74" t="s">
         <v>574</v>
       </c>
-      <c r="F74" t="s">
-        <v>568</v>
-      </c>
       <c r="G74" t="s">
         <v>568</v>
       </c>
       <c r="H74" t="s">
+        <v>568</v>
+      </c>
+      <c r="I74" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4617,17 +4636,17 @@
       <c r="E75" t="s">
         <v>573</v>
       </c>
-      <c r="F75" t="s">
-        <v>569</v>
-      </c>
       <c r="G75" t="s">
         <v>569</v>
       </c>
       <c r="H75" t="s">
+        <v>569</v>
+      </c>
+      <c r="I75" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4643,17 +4662,17 @@
       <c r="E76" t="s">
         <v>573</v>
       </c>
-      <c r="F76" t="s">
-        <v>569</v>
-      </c>
       <c r="G76" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H76" t="s">
+        <v>568</v>
+      </c>
+      <c r="I76" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4669,17 +4688,17 @@
       <c r="E77" t="s">
         <v>574</v>
       </c>
-      <c r="F77" t="s">
-        <v>568</v>
-      </c>
       <c r="G77" t="s">
         <v>568</v>
       </c>
       <c r="H77" t="s">
+        <v>568</v>
+      </c>
+      <c r="I77" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4695,17 +4714,17 @@
       <c r="E78" t="s">
         <v>574</v>
       </c>
-      <c r="F78" t="s">
-        <v>568</v>
-      </c>
       <c r="G78" t="s">
         <v>568</v>
       </c>
       <c r="H78" t="s">
+        <v>568</v>
+      </c>
+      <c r="I78" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4721,17 +4740,18 @@
       <c r="E79" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G79" t="s">
-        <v>569</v>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H79" t="s">
+        <v>569</v>
+      </c>
+      <c r="I79" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4747,17 +4767,18 @@
       <c r="E80" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G80" t="s">
-        <v>569</v>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H80" t="s">
+        <v>569</v>
+      </c>
+      <c r="I80" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4773,17 +4794,18 @@
       <c r="E81" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G81" t="s">
-        <v>569</v>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H81" t="s">
+        <v>569</v>
+      </c>
+      <c r="I81" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4799,17 +4821,18 @@
       <c r="E82" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G82" t="s">
+      <c r="F82" s="1"/>
+      <c r="G82" s="1" t="s">
         <v>568</v>
       </c>
       <c r="H82" t="s">
+        <v>568</v>
+      </c>
+      <c r="I82" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4825,17 +4848,17 @@
       <c r="E83" t="s">
         <v>575</v>
       </c>
-      <c r="F83" t="s">
-        <v>568</v>
-      </c>
       <c r="G83" t="s">
         <v>568</v>
       </c>
       <c r="H83" t="s">
+        <v>568</v>
+      </c>
+      <c r="I83" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4851,17 +4874,17 @@
       <c r="E84" t="s">
         <v>574</v>
       </c>
-      <c r="F84" t="s">
-        <v>568</v>
-      </c>
       <c r="G84" t="s">
         <v>568</v>
       </c>
       <c r="H84" t="s">
+        <v>568</v>
+      </c>
+      <c r="I84" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4877,17 +4900,17 @@
       <c r="E85" t="s">
         <v>575</v>
       </c>
-      <c r="F85" t="s">
-        <v>568</v>
-      </c>
       <c r="G85" t="s">
         <v>568</v>
       </c>
       <c r="H85" t="s">
+        <v>568</v>
+      </c>
+      <c r="I85" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4903,17 +4926,17 @@
       <c r="E86" t="s">
         <v>575</v>
       </c>
-      <c r="F86" t="s">
-        <v>568</v>
-      </c>
       <c r="G86" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H86" t="s">
+        <v>569</v>
+      </c>
+      <c r="I86" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4929,17 +4952,17 @@
       <c r="E87" t="s">
         <v>573</v>
       </c>
-      <c r="F87" t="s">
-        <v>569</v>
-      </c>
       <c r="G87" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H87" t="s">
+        <v>568</v>
+      </c>
+      <c r="I87" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4955,17 +4978,17 @@
       <c r="E88" t="s">
         <v>573</v>
       </c>
-      <c r="F88" t="s">
-        <v>569</v>
-      </c>
       <c r="G88" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H88" t="s">
+        <v>568</v>
+      </c>
+      <c r="I88" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4981,17 +5004,17 @@
       <c r="E89" t="s">
         <v>573</v>
       </c>
-      <c r="F89" t="s">
-        <v>569</v>
-      </c>
       <c r="G89" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H89" t="s">
+        <v>568</v>
+      </c>
+      <c r="I89" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5007,17 +5030,17 @@
       <c r="E90" t="s">
         <v>574</v>
       </c>
-      <c r="F90" t="s">
-        <v>568</v>
-      </c>
       <c r="G90" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H90" t="s">
+        <v>569</v>
+      </c>
+      <c r="I90" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5033,17 +5056,17 @@
       <c r="E91" t="s">
         <v>573</v>
       </c>
-      <c r="F91" t="s">
-        <v>569</v>
-      </c>
       <c r="G91" t="s">
         <v>569</v>
       </c>
       <c r="H91" t="s">
+        <v>569</v>
+      </c>
+      <c r="I91" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5059,17 +5082,17 @@
       <c r="E92" t="s">
         <v>574</v>
       </c>
-      <c r="F92" t="s">
-        <v>568</v>
-      </c>
       <c r="G92" t="s">
         <v>568</v>
       </c>
       <c r="H92" t="s">
+        <v>568</v>
+      </c>
+      <c r="I92" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5085,17 +5108,18 @@
       <c r="E93" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G93" t="s">
-        <v>569</v>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H93" t="s">
+        <v>569</v>
+      </c>
+      <c r="I93" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5111,17 +5135,18 @@
       <c r="E94" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G94" t="s">
-        <v>569</v>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H94" t="s">
+        <v>569</v>
+      </c>
+      <c r="I94" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5137,17 +5162,17 @@
       <c r="E95" t="s">
         <v>575</v>
       </c>
-      <c r="F95" t="s">
-        <v>568</v>
-      </c>
       <c r="G95" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H95" t="s">
+        <v>569</v>
+      </c>
+      <c r="I95" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5163,17 +5188,17 @@
       <c r="E96" t="s">
         <v>574</v>
       </c>
-      <c r="F96" t="s">
-        <v>568</v>
-      </c>
       <c r="G96" t="s">
         <v>568</v>
       </c>
       <c r="H96" t="s">
+        <v>568</v>
+      </c>
+      <c r="I96" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5189,17 +5214,17 @@
       <c r="E97" t="s">
         <v>574</v>
       </c>
-      <c r="F97" t="s">
-        <v>568</v>
-      </c>
       <c r="G97" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H97" t="s">
+        <v>569</v>
+      </c>
+      <c r="I97" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5215,17 +5240,17 @@
       <c r="E98" t="s">
         <v>574</v>
       </c>
-      <c r="F98" t="s">
-        <v>568</v>
-      </c>
       <c r="G98" t="s">
         <v>568</v>
       </c>
       <c r="H98" t="s">
+        <v>568</v>
+      </c>
+      <c r="I98" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5241,17 +5266,17 @@
       <c r="E99" t="s">
         <v>574</v>
       </c>
-      <c r="F99" t="s">
-        <v>568</v>
-      </c>
       <c r="G99" t="s">
         <v>568</v>
       </c>
       <c r="H99" t="s">
+        <v>568</v>
+      </c>
+      <c r="I99" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5267,17 +5292,17 @@
       <c r="E100" t="s">
         <v>574</v>
       </c>
-      <c r="F100" t="s">
-        <v>568</v>
-      </c>
       <c r="G100" t="s">
         <v>568</v>
       </c>
       <c r="H100" t="s">
+        <v>568</v>
+      </c>
+      <c r="I100" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5293,17 +5318,18 @@
       <c r="E101" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G101" t="s">
-        <v>569</v>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H101" t="s">
+        <v>569</v>
+      </c>
+      <c r="I101" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5319,17 +5345,17 @@
       <c r="E102" t="s">
         <v>575</v>
       </c>
-      <c r="F102" t="s">
-        <v>568</v>
-      </c>
       <c r="G102" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H102" t="s">
+        <v>569</v>
+      </c>
+      <c r="I102" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5345,17 +5371,17 @@
       <c r="E103" t="s">
         <v>575</v>
       </c>
-      <c r="F103" t="s">
-        <v>568</v>
-      </c>
       <c r="G103" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H103" t="s">
+        <v>569</v>
+      </c>
+      <c r="I103" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5371,17 +5397,17 @@
       <c r="E104" t="s">
         <v>574</v>
       </c>
-      <c r="F104" t="s">
-        <v>568</v>
-      </c>
       <c r="G104" t="s">
         <v>568</v>
       </c>
       <c r="H104" t="s">
+        <v>568</v>
+      </c>
+      <c r="I104" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5397,17 +5423,17 @@
       <c r="E105" t="s">
         <v>575</v>
       </c>
-      <c r="F105" t="s">
-        <v>568</v>
-      </c>
       <c r="G105" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H105" t="s">
+        <v>569</v>
+      </c>
+      <c r="I105" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5423,17 +5449,17 @@
       <c r="E106" t="s">
         <v>573</v>
       </c>
-      <c r="F106" t="s">
-        <v>569</v>
-      </c>
       <c r="G106" t="s">
         <v>569</v>
       </c>
       <c r="H106" t="s">
+        <v>569</v>
+      </c>
+      <c r="I106" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5449,17 +5475,17 @@
       <c r="E107" t="s">
         <v>573</v>
       </c>
-      <c r="F107" t="s">
-        <v>569</v>
-      </c>
       <c r="G107" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H107" t="s">
+        <v>568</v>
+      </c>
+      <c r="I107" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5475,17 +5501,17 @@
       <c r="E108" t="s">
         <v>575</v>
       </c>
-      <c r="F108" t="s">
-        <v>568</v>
-      </c>
       <c r="G108" t="s">
         <v>568</v>
       </c>
       <c r="H108" t="s">
+        <v>568</v>
+      </c>
+      <c r="I108" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5501,17 +5527,17 @@
       <c r="E109" t="s">
         <v>575</v>
       </c>
-      <c r="F109" t="s">
-        <v>568</v>
-      </c>
       <c r="G109" t="s">
         <v>568</v>
       </c>
       <c r="H109" t="s">
+        <v>568</v>
+      </c>
+      <c r="I109" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5527,17 +5553,17 @@
       <c r="E110" t="s">
         <v>575</v>
       </c>
-      <c r="F110" t="s">
-        <v>568</v>
-      </c>
       <c r="G110" t="s">
         <v>568</v>
       </c>
       <c r="H110" t="s">
+        <v>568</v>
+      </c>
+      <c r="I110" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5553,17 +5579,17 @@
       <c r="E111" t="s">
         <v>575</v>
       </c>
-      <c r="F111" t="s">
-        <v>568</v>
-      </c>
       <c r="G111" t="s">
         <v>568</v>
       </c>
       <c r="H111" t="s">
+        <v>568</v>
+      </c>
+      <c r="I111" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5579,17 +5605,17 @@
       <c r="E112" t="s">
         <v>575</v>
       </c>
-      <c r="F112" t="s">
-        <v>568</v>
-      </c>
       <c r="G112" t="s">
         <v>568</v>
       </c>
       <c r="H112" t="s">
+        <v>568</v>
+      </c>
+      <c r="I112" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5605,17 +5631,17 @@
       <c r="E113" t="s">
         <v>575</v>
       </c>
-      <c r="F113" t="s">
-        <v>568</v>
-      </c>
       <c r="G113" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H113" t="s">
+        <v>569</v>
+      </c>
+      <c r="I113" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5631,17 +5657,17 @@
       <c r="E114" t="s">
         <v>573</v>
       </c>
-      <c r="F114" t="s">
-        <v>569</v>
-      </c>
       <c r="G114" t="s">
         <v>569</v>
       </c>
       <c r="H114" t="s">
+        <v>569</v>
+      </c>
+      <c r="I114" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5657,17 +5683,17 @@
       <c r="E115" t="s">
         <v>574</v>
       </c>
-      <c r="F115" t="s">
-        <v>568</v>
-      </c>
       <c r="G115" t="s">
         <v>568</v>
       </c>
       <c r="H115" t="s">
+        <v>568</v>
+      </c>
+      <c r="I115" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5683,17 +5709,17 @@
       <c r="E116" t="s">
         <v>574</v>
       </c>
-      <c r="F116" t="s">
-        <v>568</v>
-      </c>
       <c r="G116" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H116" t="s">
+        <v>569</v>
+      </c>
+      <c r="I116" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5709,17 +5735,17 @@
       <c r="E117" t="s">
         <v>574</v>
       </c>
-      <c r="F117" t="s">
-        <v>568</v>
-      </c>
       <c r="G117" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H117" t="s">
+        <v>569</v>
+      </c>
+      <c r="I117" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5735,17 +5761,17 @@
       <c r="E118" t="s">
         <v>574</v>
       </c>
-      <c r="F118" t="s">
-        <v>568</v>
-      </c>
       <c r="G118" t="s">
         <v>568</v>
       </c>
       <c r="H118" t="s">
+        <v>568</v>
+      </c>
+      <c r="I118" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5761,17 +5787,17 @@
       <c r="E119" t="s">
         <v>574</v>
       </c>
-      <c r="F119" t="s">
-        <v>568</v>
-      </c>
       <c r="G119" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H119" t="s">
+        <v>569</v>
+      </c>
+      <c r="I119" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5787,17 +5813,17 @@
       <c r="E120" t="s">
         <v>574</v>
       </c>
-      <c r="F120" t="s">
-        <v>568</v>
-      </c>
       <c r="G120" t="s">
         <v>568</v>
       </c>
       <c r="H120" t="s">
+        <v>568</v>
+      </c>
+      <c r="I120" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5813,17 +5839,17 @@
       <c r="E121" t="s">
         <v>574</v>
       </c>
-      <c r="F121" t="s">
-        <v>568</v>
-      </c>
       <c r="G121" t="s">
         <v>568</v>
       </c>
       <c r="H121" t="s">
+        <v>568</v>
+      </c>
+      <c r="I121" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5839,17 +5865,17 @@
       <c r="E122" t="s">
         <v>575</v>
       </c>
-      <c r="F122" t="s">
-        <v>568</v>
-      </c>
       <c r="G122" t="s">
         <v>568</v>
       </c>
       <c r="H122" t="s">
+        <v>568</v>
+      </c>
+      <c r="I122" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5865,17 +5891,17 @@
       <c r="E123" t="s">
         <v>574</v>
       </c>
-      <c r="F123" t="s">
-        <v>568</v>
-      </c>
       <c r="G123" t="s">
         <v>568</v>
       </c>
       <c r="H123" t="s">
+        <v>568</v>
+      </c>
+      <c r="I123" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5891,17 +5917,18 @@
       <c r="E124" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F124" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G124" t="s">
-        <v>569</v>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H124" t="s">
+        <v>569</v>
+      </c>
+      <c r="I124" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5917,17 +5944,18 @@
       <c r="E125" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G125" t="s">
-        <v>569</v>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H125" t="s">
+        <v>569</v>
+      </c>
+      <c r="I125" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5943,17 +5971,17 @@
       <c r="E126" t="s">
         <v>575</v>
       </c>
-      <c r="F126" t="s">
-        <v>568</v>
-      </c>
       <c r="G126" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H126" t="s">
+        <v>569</v>
+      </c>
+      <c r="I126" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5969,17 +5997,17 @@
       <c r="E127" t="s">
         <v>574</v>
       </c>
-      <c r="F127" t="s">
-        <v>568</v>
-      </c>
       <c r="G127" t="s">
         <v>568</v>
       </c>
       <c r="H127" t="s">
+        <v>568</v>
+      </c>
+      <c r="I127" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5995,17 +6023,17 @@
       <c r="E128" t="s">
         <v>574</v>
       </c>
-      <c r="F128" t="s">
-        <v>568</v>
-      </c>
       <c r="G128" t="s">
         <v>568</v>
       </c>
       <c r="H128" t="s">
+        <v>568</v>
+      </c>
+      <c r="I128" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -6021,17 +6049,17 @@
       <c r="E129" t="s">
         <v>573</v>
       </c>
-      <c r="F129" t="s">
-        <v>569</v>
-      </c>
       <c r="G129" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H129" t="s">
+        <v>568</v>
+      </c>
+      <c r="I129" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -6047,17 +6075,17 @@
       <c r="E130" t="s">
         <v>573</v>
       </c>
-      <c r="F130" t="s">
-        <v>569</v>
-      </c>
       <c r="G130" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H130" t="s">
+        <v>568</v>
+      </c>
+      <c r="I130" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -6073,17 +6101,18 @@
       <c r="E131" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F131" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G131" t="s">
-        <v>569</v>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H131" t="s">
+        <v>569</v>
+      </c>
+      <c r="I131" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -6099,17 +6128,17 @@
       <c r="E132" t="s">
         <v>574</v>
       </c>
-      <c r="F132" t="s">
-        <v>568</v>
-      </c>
       <c r="G132" t="s">
         <v>568</v>
       </c>
       <c r="H132" t="s">
+        <v>568</v>
+      </c>
+      <c r="I132" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -6125,17 +6154,17 @@
       <c r="E133" t="s">
         <v>575</v>
       </c>
-      <c r="F133" t="s">
-        <v>568</v>
-      </c>
       <c r="G133" t="s">
         <v>568</v>
       </c>
       <c r="H133" t="s">
+        <v>568</v>
+      </c>
+      <c r="I133" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -6151,17 +6180,18 @@
       <c r="E134" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F134" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G134" t="s">
-        <v>569</v>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H134" t="s">
+        <v>569</v>
+      </c>
+      <c r="I134" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -6177,17 +6207,17 @@
       <c r="E135" t="s">
         <v>573</v>
       </c>
-      <c r="F135" t="s">
-        <v>569</v>
-      </c>
       <c r="G135" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H135" t="s">
+        <v>568</v>
+      </c>
+      <c r="I135" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -6203,17 +6233,17 @@
       <c r="E136" t="s">
         <v>573</v>
       </c>
-      <c r="F136" t="s">
-        <v>569</v>
-      </c>
       <c r="G136" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H136" t="s">
+        <v>568</v>
+      </c>
+      <c r="I136" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -6229,17 +6259,17 @@
       <c r="E137" t="s">
         <v>573</v>
       </c>
-      <c r="F137" t="s">
-        <v>569</v>
-      </c>
       <c r="G137" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H137" t="s">
+        <v>568</v>
+      </c>
+      <c r="I137" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -6255,17 +6285,17 @@
       <c r="E138" t="s">
         <v>575</v>
       </c>
-      <c r="F138" t="s">
-        <v>568</v>
-      </c>
       <c r="G138" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H138" t="s">
+        <v>569</v>
+      </c>
+      <c r="I138" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -6281,17 +6311,17 @@
       <c r="E139" t="s">
         <v>573</v>
       </c>
-      <c r="F139" t="s">
-        <v>569</v>
-      </c>
       <c r="G139" t="s">
         <v>569</v>
       </c>
       <c r="H139" t="s">
+        <v>569</v>
+      </c>
+      <c r="I139" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -6307,17 +6337,18 @@
       <c r="E140" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F140" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G140" t="s">
+      <c r="F140" s="1"/>
+      <c r="G140" s="1" t="s">
         <v>568</v>
       </c>
       <c r="H140" t="s">
+        <v>568</v>
+      </c>
+      <c r="I140" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -6333,17 +6364,18 @@
       <c r="E141" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F141" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G141" t="s">
-        <v>569</v>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H141" t="s">
+        <v>569</v>
+      </c>
+      <c r="I141" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -6359,17 +6391,17 @@
       <c r="E142" t="s">
         <v>573</v>
       </c>
-      <c r="F142" t="s">
-        <v>569</v>
-      </c>
       <c r="G142" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H142" t="s">
+        <v>568</v>
+      </c>
+      <c r="I142" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -6385,17 +6417,17 @@
       <c r="E143" t="s">
         <v>573</v>
       </c>
-      <c r="F143" t="s">
-        <v>569</v>
-      </c>
       <c r="G143" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H143" t="s">
+        <v>568</v>
+      </c>
+      <c r="I143" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -6411,17 +6443,17 @@
       <c r="E144" t="s">
         <v>573</v>
       </c>
-      <c r="F144" t="s">
-        <v>569</v>
-      </c>
       <c r="G144" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H144" t="s">
+        <v>568</v>
+      </c>
+      <c r="I144" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -6437,17 +6469,18 @@
       <c r="E145" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F145" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G145" t="s">
-        <v>569</v>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H145" t="s">
+        <v>569</v>
+      </c>
+      <c r="I145" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -6463,17 +6496,18 @@
       <c r="E146" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="F146" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="G146" t="s">
-        <v>569</v>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="H146" t="s">
+        <v>569</v>
+      </c>
+      <c r="I146" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -6489,17 +6523,17 @@
       <c r="E147" t="s">
         <v>573</v>
       </c>
-      <c r="F147" t="s">
-        <v>569</v>
-      </c>
       <c r="G147" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H147" t="s">
+        <v>568</v>
+      </c>
+      <c r="I147" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -6515,17 +6549,17 @@
       <c r="E148" t="s">
         <v>574</v>
       </c>
-      <c r="F148" t="s">
-        <v>568</v>
-      </c>
       <c r="G148" t="s">
         <v>568</v>
       </c>
       <c r="H148" t="s">
+        <v>568</v>
+      </c>
+      <c r="I148" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -6541,17 +6575,17 @@
       <c r="E149" t="s">
         <v>575</v>
       </c>
-      <c r="F149" t="s">
-        <v>568</v>
-      </c>
       <c r="G149" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H149" t="s">
+        <v>569</v>
+      </c>
+      <c r="I149" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -6567,18 +6601,18 @@
       <c r="E150" t="s">
         <v>575</v>
       </c>
-      <c r="F150" t="s">
-        <v>568</v>
-      </c>
       <c r="G150" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H150" t="s">
+        <v>569</v>
+      </c>
+      <c r="I150" t="s">
         <v>444</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H150">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I150">
     <sortCondition ref="A2:A150"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
#38 update Boolean, DatasetType, Date, and Spatial Reference
</commit_message>
<xml_diff>
--- a/resources/parameters.xlsx
+++ b/resources/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlhumber/iiipy/autobox/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19F438D-F886-6445-8DF2-7E4718F27DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C726371D-E59F-9740-A25F-6A6C3A6F6689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C9864FCB-DD2E-D646-9669-B24A34CEB34F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="577">
   <si>
     <t>3D Tiles Layer</t>
   </si>
@@ -2881,11 +2881,14 @@
       <c r="E8" t="s">
         <v>574</v>
       </c>
+      <c r="F8" t="s">
+        <v>575</v>
+      </c>
       <c r="G8" t="s">
         <v>568</v>
       </c>
       <c r="H8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I8" t="s">
         <v>20</v>
@@ -3298,11 +3301,14 @@
       <c r="E24" t="s">
         <v>574</v>
       </c>
+      <c r="F24" t="s">
+        <v>575</v>
+      </c>
       <c r="G24" t="s">
         <v>568</v>
       </c>
       <c r="H24" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I24" t="s">
         <v>68</v>
@@ -3324,11 +3330,14 @@
       <c r="E25" t="s">
         <v>574</v>
       </c>
+      <c r="F25" t="s">
+        <v>575</v>
+      </c>
       <c r="G25" t="s">
         <v>568</v>
       </c>
       <c r="H25" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I25" t="s">
         <v>71</v>
@@ -5709,11 +5718,14 @@
       <c r="E116" t="s">
         <v>574</v>
       </c>
+      <c r="F116" t="s">
+        <v>575</v>
+      </c>
       <c r="G116" t="s">
         <v>568</v>
       </c>
       <c r="H116" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I116" t="s">
         <v>342</v>

</xml_diff>